<commit_message>
update evaluations forms - Brioche
</commit_message>
<xml_diff>
--- a/Evaluations Forms/EvaluationForms-W__-38200127-BriocheLiuKangjie.xlsx
+++ b/Evaluations Forms/EvaluationForms-W__-38200127-BriocheLiuKangjie.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20338"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brioche\Desktop\dsd_dbest\Evaluations Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utad4-my.sharepoint.com/personal/al22653_alunos_utad_pt/Documents/Ambiente de Trabalho/Evaluations Week 1/Evaluations Forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8EE680-381C-49F7-92F6-6DC333061FED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{79439C10-66A9-4863-AD7A-79C26F75526D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D708EBC6-E6D5-4597-94F3-315BF73CA654}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21375" windowHeight="6855" xr2:uid="{C837394A-674A-4B62-AC40-90A56BBDFD1D}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{C837394A-674A-4B62-AC40-90A56BBDFD1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Member" sheetId="1" r:id="rId1"/>
+    <sheet name="Team" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Contribution</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -87,6 +99,27 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Team work load completed in respect of the whole project.</t>
+  </si>
+  <si>
+    <t>List all the other teams other than your own team.</t>
+  </si>
+  <si>
+    <t>The module that team is responsible for.</t>
+  </si>
+  <si>
+    <t>Team performance in the inter-team collaboration.</t>
+  </si>
+  <si>
+    <t>Effective and timely communication with other teams.</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
     <t>Inner Team Assessment（1~5）</t>
   </si>
   <si>
@@ -114,6 +147,18 @@
     <t>Summary</t>
   </si>
   <si>
+    <t>Inter Team Assessment（1~10）</t>
+  </si>
+  <si>
+    <t>Team Name</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Liveness</t>
+  </si>
+  <si>
     <t>Database Developers</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -126,10 +171,44 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Database Architect</t>
-  </si>
-  <si>
-    <t>Bill</t>
+    <t>Infrastructure Tester</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mvp</t>
+  </si>
+  <si>
+    <t>genshin-impact</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>mihoyo</t>
+  </si>
+  <si>
+    <t>dreamweaver</t>
+  </si>
+  <si>
+    <t>pi_rates</t>
+  </si>
+  <si>
+    <t>Brioche</t>
+  </si>
+  <si>
+    <t>Database Engineer</t>
+  </si>
+  <si>
+    <t>Webpage</t>
+  </si>
+  <si>
+    <t>Algorithms (AI)</t>
+  </si>
+  <si>
+    <t>Mobile App</t>
+  </si>
+  <si>
+    <t>Sensors</t>
   </si>
   <si>
     <t xml:space="preserve">Team Leader </t>
@@ -145,20 +224,17 @@
   </si>
   <si>
     <t>Maxwell</t>
-  </si>
-  <si>
-    <t>Infrastructure Tester</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -166,21 +242,21 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -188,7 +264,7 @@
     <font>
       <sz val="11"/>
       <color theme="2"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -240,8 +316,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -259,18 +338,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -285,8 +367,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -584,27 +670,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C98B110-97C1-4E21-93A3-ADA4289AC304}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="5.75" style="2"/>
+    <col min="1" max="1" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="5.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -614,251 +700,251 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="1">
+      <c r="J1" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
+    <row r="2" spans="1:11" ht="15" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="G2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="2">
         <v>2</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:11" ht="15" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="4">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4">
+        <v>5</v>
+      </c>
+      <c r="I3" s="4">
+        <f>SUM(C3:H3)</f>
         <v>30</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="3">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3">
-        <v>5</v>
-      </c>
-      <c r="F3" s="3">
-        <v>5</v>
-      </c>
-      <c r="G3" s="3">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3">
-        <v>5</v>
-      </c>
-      <c r="I3" s="3">
-        <f t="shared" ref="I3:I8" si="0">SUM(C3:H3)</f>
+      <c r="J3" s="2"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4">
+        <f>SUM(C4:H4)</f>
         <v>30</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="3">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3">
-        <v>5</v>
-      </c>
-      <c r="F4" s="3">
-        <v>5</v>
-      </c>
-      <c r="G4" s="3">
-        <v>5</v>
-      </c>
-      <c r="H4" s="3">
-        <v>5</v>
-      </c>
-      <c r="I4" s="6">
+      <c r="J4" s="2">
+        <v>3</v>
+      </c>
+      <c r="K4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4">
+        <v>5</v>
+      </c>
+      <c r="G5" s="4">
+        <v>5</v>
+      </c>
+      <c r="H5" s="4">
+        <v>5</v>
+      </c>
+      <c r="I5" s="4">
+        <f>SUM(C5:H5)</f>
+        <v>30</v>
+      </c>
+      <c r="J5" s="2">
+        <v>4</v>
+      </c>
+      <c r="K5" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1">
+      <c r="A6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" ref="I6:I8" si="0">SUM(C6:H6)</f>
+        <v>30</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1">
+      <c r="A7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J4" s="1">
-        <v>3</v>
-      </c>
-      <c r="K4" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="3">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3">
-        <v>5</v>
-      </c>
-      <c r="E5" s="3">
-        <v>5</v>
-      </c>
-      <c r="F5" s="3">
-        <v>5</v>
-      </c>
-      <c r="G5" s="3">
-        <v>5</v>
-      </c>
-      <c r="H5" s="3">
-        <v>5</v>
-      </c>
-      <c r="I5" s="6">
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1">
+      <c r="A8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4">
+        <v>5</v>
+      </c>
+      <c r="H8" s="4">
+        <v>5</v>
+      </c>
+      <c r="I8" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="3">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3">
-        <v>5</v>
-      </c>
-      <c r="F6" s="3">
-        <v>5</v>
-      </c>
-      <c r="G6" s="3">
-        <v>5</v>
-      </c>
-      <c r="H6" s="3">
-        <v>5</v>
-      </c>
-      <c r="I6" s="6">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="J6" s="1">
-        <v>4</v>
-      </c>
-      <c r="K6" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>5</v>
-      </c>
-      <c r="G7" s="3">
-        <v>5</v>
-      </c>
-      <c r="H7" s="3">
-        <v>5</v>
-      </c>
-      <c r="I7" s="6">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="J7" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="6">
-        <v>5</v>
-      </c>
-      <c r="D8" s="6">
-        <v>5</v>
-      </c>
-      <c r="E8" s="6">
-        <v>5</v>
-      </c>
-      <c r="F8" s="6">
-        <v>5</v>
-      </c>
-      <c r="G8" s="6">
-        <v>5</v>
-      </c>
-      <c r="H8" s="6">
-        <v>5</v>
-      </c>
-      <c r="I8" s="6">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="9" spans="1:11" ht="15" customHeight="1"/>
+    <row r="10" spans="1:11" ht="15" customHeight="1">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:11" ht="15" customHeight="1">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -872,8 +958,8 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:11" ht="15" customHeight="1">
+      <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -887,8 +973,8 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:11" ht="15" customHeight="1">
+      <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -902,8 +988,8 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:11" ht="15" customHeight="1">
+      <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -917,8 +1003,8 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:11" ht="15" customHeight="1">
+      <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -932,8 +1018,8 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:11" ht="15" customHeight="1">
+      <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -947,8 +1033,8 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:9" ht="15" customHeight="1">
+      <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -975,11 +1061,257 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:H7 C8:H8" xr:uid="{E638E43E-6F1C-4712-A08C-EBD677F4902A}">
-      <formula1>$J$1:$J$7</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:H9" xr:uid="{E638E43E-6F1C-4712-A08C-EBD677F4902A}">
+      <formula1>$J$1:$J$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99BAAD3A-F151-4ADE-B12F-ECC415EB594F}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="J1" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <f>SUM(C3:E3)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <f>SUM(C4:E4)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <f>SUM(C5:E5)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <f>SUM(C6:E6)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <f>SUM(C7:E7)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B13:H13"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>